<commit_message>
Review SRS_User Transactions Module and update coach review sheet format
</commit_message>
<xml_diff>
--- a/Project Management/PM_Coaching_Review.xlsx
+++ b/Project Management/PM_Coaching_Review.xlsx
@@ -1,79 +1,217 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Quality Assurance\Internal-Banking-System\Project Management\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="الورقة1" sheetId="1" r:id="rId4"/>
+    <sheet name="الورقة1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t xml:space="preserve">release version </t>
-  </si>
-  <si>
-    <t>comments</t>
-  </si>
-  <si>
-    <t>time</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>revision record should be added to PMP</t>
+  </si>
+  <si>
+    <t>Esraa</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>release strategy should be added to PMP</t>
+  </si>
+  <si>
+    <t>baseline strategy should be added to PMP</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>tuesdays meetings should be added to pmp</t>
+  </si>
+  <si>
+    <t>Mohammed Hassan</t>
+  </si>
+  <si>
+    <t>page 4 issues tracking record should be added to PMP</t>
+  </si>
+  <si>
+    <t>esclation process should be added to PMP</t>
+  </si>
+  <si>
+    <t>update folder structure in CIL</t>
+  </si>
+  <si>
+    <t>internal change request should be mentioned in PMP</t>
+  </si>
+  <si>
+    <t>commit message need to be clear</t>
+  </si>
+  <si>
+    <t>add review phase between inprogress and finish in trello</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Release
+version </t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -263,36 +401,297 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AR17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="26.25"/>
-    <col customWidth="1" min="2" max="2" width="28.63"/>
-    <col customWidth="1" min="3" max="3" width="26.88"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="52.6640625" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:44" s="7" customFormat="1" ht="51.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="8"/>
+      <c r="AL1" s="8"/>
+      <c r="AM1" s="8"/>
+      <c r="AN1" s="8"/>
+      <c r="AO1" s="8"/>
+      <c r="AP1" s="8"/>
+      <c r="AQ1" s="8"/>
+      <c r="AR1" s="8"/>
+    </row>
+    <row r="2" spans="1:44" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>45380</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44" s="1" customFormat="1" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3">
+        <v>45380</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:44" s="1" customFormat="1" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45380</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:44" s="1" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45381</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:44" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3">
+        <v>45381</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:44" s="1" customFormat="1" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3">
+        <v>45381</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44" s="1" customFormat="1" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45381</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:44" s="1" customFormat="1" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="3">
+        <v>45381</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:44" s="1" customFormat="1" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="3">
+        <v>45381</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:44" s="1" customFormat="1" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="3">
+        <v>45381</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:44" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:44" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:44" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:44" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:44" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding the User Transaction feature SIQ and SRS
</commit_message>
<xml_diff>
--- a/Project Management/PM_Coaching_Review.xlsx
+++ b/Project Management/PM_Coaching_Review.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="130" yWindow="560" windowWidth="18880" windowHeight="6740"/>
   </bookViews>
   <sheets>
-    <sheet name="الورقة1" sheetId="1" r:id="rId1"/>
+    <sheet name="coaching Review" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="28">
   <si>
     <t>Number</t>
   </si>
@@ -83,7 +83,25 @@
 version </t>
   </si>
   <si>
-    <t>V1</t>
+    <t>release name doesn't follow the release naming
+ convension as mensioned in PMP</t>
+  </si>
+  <si>
+    <t>17/4/2024</t>
+  </si>
+  <si>
+    <t>V1.0</t>
+  </si>
+  <si>
+    <t>V2.0</t>
+  </si>
+  <si>
+    <t>in [Req_SIQ]: the second tab should be named 
+"Revision Record" not Report.</t>
+  </si>
+  <si>
+    <t>Why is there REQ_SIQ and REQ_SIQ_Responses
+ not only one sheet?</t>
   </si>
 </sst>
 </file>
@@ -140,13 +158,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -364,16 +385,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.26953125" customWidth="1"/>
-    <col min="2" max="2" width="28.6328125" customWidth="1"/>
+    <col min="2" max="2" width="40.90625" customWidth="1"/>
     <col min="3" max="3" width="26.90625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -414,7 +435,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -434,7 +455,7 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -454,7 +475,7 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -474,7 +495,7 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -494,7 +515,7 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -514,7 +535,7 @@
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -534,7 +555,7 @@
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -554,7 +575,7 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -574,7 +595,7 @@
         <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -594,7 +615,67 @@
         <v>8</v>
       </c>
       <c r="F11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="48.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding High Level Designs
</commit_message>
<xml_diff>
--- a/Project Management/PM_Coaching_Review.xlsx
+++ b/Project Management/PM_Coaching_Review.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="32">
   <si>
     <t>Number</t>
   </si>
@@ -102,6 +102,18 @@
   <si>
     <t>Why is there REQ_SIQ and REQ_SIQ_Responses
  not only one sheet?</t>
+  </si>
+  <si>
+    <t>account/user deletion criteria must be mentioned</t>
+  </si>
+  <si>
+    <t>20/4/2024</t>
+  </si>
+  <si>
+    <t>opened</t>
+  </si>
+  <si>
+    <t>V3.0</t>
   </si>
 </sst>
 </file>
@@ -385,10 +397,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -678,6 +690,26 @@
         <v>25</v>
       </c>
     </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
changing ID names of User Transactions in SIQ,SRS,RTM & user/account deletion criteria has been mentioed
</commit_message>
<xml_diff>
--- a/Project Management/PM_Coaching_Review.xlsx
+++ b/Project Management/PM_Coaching_Review.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="31">
   <si>
     <t>Number</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>20/4/2024</t>
-  </si>
-  <si>
-    <t>opened</t>
   </si>
   <si>
     <t>V3.0</t>
@@ -400,7 +397,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -704,10 +701,10 @@
         <v>14</v>
       </c>
       <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
         <v>30</v>
-      </c>
-      <c r="F15" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>